<commit_message>
Made a Mannings Rating Curve module
I think it works?
</commit_message>
<xml_diff>
--- a/Data/Q/R2_HEC.xlsx
+++ b/Data/Q/R2_HEC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="HEC4" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="DT Upstream" sheetId="5" r:id="rId5"/>
     <sheet name="DT Downstream" sheetId="6" r:id="rId6"/>
     <sheet name="Summary" sheetId="7" r:id="rId7"/>
+    <sheet name="Summary_m" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="32">
   <si>
     <t>Dist</t>
   </si>
@@ -104,7 +105,28 @@
     <t>RB</t>
   </si>
   <si>
-    <t>S</t>
+    <t>HEC Cross Section</t>
+  </si>
+  <si>
+    <t>Measured Cross Section</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>Elevation</t>
+  </si>
+  <si>
+    <t>Reach Lengths</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>RL</t>
   </si>
 </sst>
 </file>
@@ -115,7 +137,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +161,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -154,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -201,11 +231,150 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -224,6 +393,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,11 +611,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="304307096"/>
-        <c:axId val="304308272"/>
+        <c:axId val="263812248"/>
+        <c:axId val="263811856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="304307096"/>
+        <c:axId val="263812248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -474,7 +658,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="304308272"/>
+        <c:crossAx val="263811856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -482,7 +666,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="304308272"/>
+        <c:axId val="263811856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -533,7 +717,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="304307096"/>
+        <c:crossAx val="263812248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -629,7 +813,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -806,11 +989,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="390542696"/>
-        <c:axId val="390541128"/>
+        <c:axId val="263813032"/>
+        <c:axId val="263812640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="390542696"/>
+        <c:axId val="263813032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -853,7 +1036,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="390541128"/>
+        <c:crossAx val="263812640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -861,7 +1044,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="390541128"/>
+        <c:axId val="263812640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -912,7 +1095,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="390542696"/>
+        <c:crossAx val="263813032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -926,7 +1109,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1008,7 +1190,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1167,11 +1348,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="304293376"/>
-        <c:axId val="304293768"/>
+        <c:axId val="263811464"/>
+        <c:axId val="263815384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="304293376"/>
+        <c:axId val="263811464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1214,7 +1395,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="304293768"/>
+        <c:crossAx val="263815384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1222,7 +1403,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="304293768"/>
+        <c:axId val="263815384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1273,7 +1454,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="304293376"/>
+        <c:crossAx val="263811464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1287,7 +1468,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1369,7 +1549,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1534,11 +1713,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="304303960"/>
-        <c:axId val="304301608"/>
+        <c:axId val="263808720"/>
+        <c:axId val="263809112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="304303960"/>
+        <c:axId val="263808720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1581,7 +1760,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="304301608"/>
+        <c:crossAx val="263809112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1589,7 +1768,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="304301608"/>
+        <c:axId val="263809112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1640,7 +1819,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="304303960"/>
+        <c:crossAx val="263808720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1654,7 +1833,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1751,7 +1929,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2180,11 +2357,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="394549608"/>
-        <c:axId val="394530008"/>
+        <c:axId val="265091936"/>
+        <c:axId val="265092328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="394549608"/>
+        <c:axId val="265091936"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2206,19 +2383,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="394530008"/>
+        <c:crossAx val="265092328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="394530008"/>
+        <c:axId val="265092328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="-60"/>
@@ -2243,14 +2419,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="394549608"/>
+        <c:crossAx val="265091936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2276,6 +2451,710 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>HEC Cross Sections - R2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Summary!$E$6:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60.96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>121.92</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>182.88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>243.84</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>253.89840000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>253.89840000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>304.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>365.76</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>373.38</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>373.38</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>401.11680000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$D$6:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>-66.040000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-86.36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-95.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-118.11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-125.73</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-122.55500000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-129.54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-148.59</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-128.27000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-144.78</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-132.08000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-137.16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-134.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Summary!$E$6:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60.96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>121.92</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>182.88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>243.84</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>253.89840000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>253.89840000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>304.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>365.76</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>373.38</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>373.38</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>401.11680000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$F$6:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>8.89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-138.43</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-154.94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-168.91</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-176.53</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-180.34</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-186.69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-193.04</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-193.04</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-199.39000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-203.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-185.42000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-99.06</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$H$6:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-93.98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-121.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-171.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-200.66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-205.74</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-185.42000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-214.63</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-224.79</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-210.82</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-185.42000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-157.47999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$J$6:$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-159.38499999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-215.26499999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-250.82499999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-255.90500000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-258.44499999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-268.60500000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-266.065</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-250.82499999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-245.745</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-230.505</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-141.60500000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-93.344999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="316657664"/>
+        <c:axId val="316655312"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="316657664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="316655312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="316655312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="316657664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2441,6 +3320,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -3951,6 +4870,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4620,6 +6042,41 @@
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4902,7 +6359,7 @@
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4915,6 +6372,9 @@
         <v>6</v>
       </c>
       <c r="C2" s="1"/>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
@@ -5293,7 +6753,7 @@
   <dimension ref="B2:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5306,6 +6766,9 @@
         <v>8</v>
       </c>
       <c r="C2" s="1"/>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
@@ -5730,7 +7193,7 @@
   <dimension ref="B2:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:H16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5743,6 +7206,9 @@
         <v>10</v>
       </c>
       <c r="C2" s="1"/>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
@@ -6109,7 +7575,7 @@
   <dimension ref="B1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:M3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6137,6 +7603,9 @@
         <v>15</v>
       </c>
       <c r="C2" s="1"/>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
       <c r="I2" t="s">
         <v>13</v>
       </c>
@@ -6679,7 +8148,7 @@
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7">
-        <f>B7*12*2.54</f>
+        <f t="shared" ref="F7:F29" si="0">B7*12*2.54</f>
         <v>0</v>
       </c>
       <c r="G7" s="7">
@@ -6687,7 +8156,7 @@
         <v>136.52500000000001</v>
       </c>
       <c r="H7" s="7">
-        <f>-G7</f>
+        <f t="shared" ref="H7:H29" si="1">-G7</f>
         <v>-136.52500000000001</v>
       </c>
     </row>
@@ -6703,15 +8172,15 @@
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7">
-        <f>B8*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>152.4</v>
       </c>
       <c r="G8" s="7">
-        <f t="shared" ref="G8:G29" si="0">((C8*12)+D8)*2.54+$M$3</f>
+        <f t="shared" ref="G8:G29" si="2">((C8*12)+D8)*2.54+$M$3</f>
         <v>146.685</v>
       </c>
       <c r="H8" s="7">
-        <f>-G8</f>
+        <f t="shared" si="1"/>
         <v>-146.685</v>
       </c>
     </row>
@@ -6727,15 +8196,15 @@
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7">
-        <f>B9*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>304.8</v>
       </c>
       <c r="G9" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>154.94</v>
       </c>
       <c r="H9" s="7">
-        <f>-G9</f>
+        <f t="shared" si="1"/>
         <v>-154.94</v>
       </c>
     </row>
@@ -6751,15 +8220,15 @@
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7">
-        <f>B10*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>457.2</v>
       </c>
       <c r="G10" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>163.82999999999998</v>
       </c>
       <c r="H10" s="7">
-        <f>-G10</f>
+        <f t="shared" si="1"/>
         <v>-163.82999999999998</v>
       </c>
     </row>
@@ -6775,15 +8244,15 @@
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7">
-        <f>B11*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>609.6</v>
       </c>
       <c r="G11" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>173.35500000000002</v>
       </c>
       <c r="H11" s="7">
-        <f>-G11</f>
+        <f t="shared" si="1"/>
         <v>-173.35500000000002</v>
       </c>
     </row>
@@ -6799,15 +8268,15 @@
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7">
-        <f>B12*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>670.56000000000006</v>
       </c>
       <c r="G12" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>180.34</v>
       </c>
       <c r="H12" s="7">
-        <f>-G12</f>
+        <f t="shared" si="1"/>
         <v>-180.34</v>
       </c>
     </row>
@@ -6826,15 +8295,15 @@
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7">
-        <f>B13*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>701.04</v>
       </c>
       <c r="G13" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>183.51500000000001</v>
       </c>
       <c r="H13" s="7">
-        <f>-G13</f>
+        <f t="shared" si="1"/>
         <v>-183.51500000000001</v>
       </c>
     </row>
@@ -6850,15 +8319,15 @@
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7">
-        <f>B14*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>762</v>
       </c>
       <c r="G14" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>189.86500000000001</v>
       </c>
       <c r="H14" s="7">
-        <f>-G14</f>
+        <f t="shared" si="1"/>
         <v>-189.86500000000001</v>
       </c>
     </row>
@@ -6874,15 +8343,15 @@
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7">
-        <f>B15*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>792.48</v>
       </c>
       <c r="G15" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>190.5</v>
       </c>
       <c r="H15" s="7">
-        <f>-G15</f>
+        <f t="shared" si="1"/>
         <v>-190.5</v>
       </c>
     </row>
@@ -6898,15 +8367,15 @@
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7">
-        <f>B16*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>822.96</v>
       </c>
       <c r="G16" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>193.04</v>
       </c>
       <c r="H16" s="7">
-        <f>-G16</f>
+        <f t="shared" si="1"/>
         <v>-193.04</v>
       </c>
     </row>
@@ -6922,15 +8391,15 @@
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7">
-        <f>B17*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>853.44</v>
       </c>
       <c r="G17" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>193.67500000000001</v>
       </c>
       <c r="H17" s="7">
-        <f>-G17</f>
+        <f t="shared" si="1"/>
         <v>-193.67500000000001</v>
       </c>
     </row>
@@ -6946,15 +8415,15 @@
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7">
-        <f>B18*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>883.92</v>
       </c>
       <c r="G18" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>191.77</v>
       </c>
       <c r="H18" s="7">
-        <f>-G18</f>
+        <f t="shared" si="1"/>
         <v>-191.77</v>
       </c>
     </row>
@@ -6970,15 +8439,15 @@
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7">
-        <f>B19*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>914.4</v>
       </c>
       <c r="G19" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>189.86500000000001</v>
       </c>
       <c r="H19" s="7">
-        <f>-G19</f>
+        <f t="shared" si="1"/>
         <v>-189.86500000000001</v>
       </c>
     </row>
@@ -6994,15 +8463,15 @@
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7">
-        <f>B20*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>944.88</v>
       </c>
       <c r="G20" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>187.32500000000002</v>
       </c>
       <c r="H20" s="7">
-        <f>-G20</f>
+        <f t="shared" si="1"/>
         <v>-187.32500000000002</v>
       </c>
     </row>
@@ -7021,15 +8490,15 @@
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7">
-        <f>B21*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1005.84</v>
       </c>
       <c r="G21" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>183.51500000000001</v>
       </c>
       <c r="H21" s="7">
-        <f>-G21</f>
+        <f t="shared" si="1"/>
         <v>-183.51500000000001</v>
       </c>
     </row>
@@ -7045,15 +8514,15 @@
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7">
-        <f>B22*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1036.32</v>
       </c>
       <c r="G22" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>180.34</v>
       </c>
       <c r="H22" s="7">
-        <f>-G22</f>
+        <f t="shared" si="1"/>
         <v>-180.34</v>
       </c>
     </row>
@@ -7069,15 +8538,15 @@
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7">
-        <f>B23*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1097.28</v>
       </c>
       <c r="G23" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>177.8</v>
       </c>
       <c r="H23" s="7">
-        <f>-G23</f>
+        <f t="shared" si="1"/>
         <v>-177.8</v>
       </c>
     </row>
@@ -7093,15 +8562,15 @@
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7">
-        <f>B24*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1158.24</v>
       </c>
       <c r="G24" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>173.35500000000002</v>
       </c>
       <c r="H24" s="7">
-        <f>-G24</f>
+        <f t="shared" si="1"/>
         <v>-173.35500000000002</v>
       </c>
     </row>
@@ -7117,15 +8586,15 @@
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7">
-        <f>B25*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1219.2</v>
       </c>
       <c r="G25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>169.54500000000002</v>
       </c>
       <c r="H25" s="7">
-        <f>-G25</f>
+        <f t="shared" si="1"/>
         <v>-169.54500000000002</v>
       </c>
     </row>
@@ -7141,15 +8610,15 @@
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7">
-        <f>B26*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1280.1600000000001</v>
       </c>
       <c r="G26" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>165.10000000000002</v>
       </c>
       <c r="H26" s="7">
-        <f>-G26</f>
+        <f t="shared" si="1"/>
         <v>-165.10000000000002</v>
       </c>
     </row>
@@ -7165,15 +8634,15 @@
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7">
-        <f>B27*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1371.6</v>
       </c>
       <c r="G27" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>162.56</v>
       </c>
       <c r="H27" s="7">
-        <f>-G27</f>
+        <f t="shared" si="1"/>
         <v>-162.56</v>
       </c>
     </row>
@@ -7189,15 +8658,15 @@
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7">
-        <f>B28*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1524</v>
       </c>
       <c r="G28" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>140.97</v>
       </c>
       <c r="H28" s="7">
-        <f>-G28</f>
+        <f t="shared" si="1"/>
         <v>-140.97</v>
       </c>
     </row>
@@ -7213,15 +8682,15 @@
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7">
-        <f>B29*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1676.4</v>
       </c>
       <c r="G29" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>120.65</v>
       </c>
       <c r="H29" s="7">
-        <f>-G29</f>
+        <f t="shared" si="1"/>
         <v>-120.65</v>
       </c>
     </row>
@@ -7363,7 +8832,7 @@
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7">
-        <f>B7*12*2.54</f>
+        <f t="shared" ref="F7:F29" si="0">B7*12*2.54</f>
         <v>0</v>
       </c>
       <c r="G7" s="7">
@@ -7371,7 +8840,7 @@
         <v>135.255</v>
       </c>
       <c r="H7" s="7">
-        <f>-G7</f>
+        <f t="shared" ref="H7:H29" si="1">-G7</f>
         <v>-135.255</v>
       </c>
     </row>
@@ -7387,15 +8856,15 @@
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7">
-        <f>B8*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>152.4</v>
       </c>
       <c r="G8" s="7">
-        <f>((C8*12)+D8)*2.54</f>
+        <f t="shared" ref="G8:G29" si="2">((C8*12)+D8)*2.54</f>
         <v>92.710000000000008</v>
       </c>
       <c r="H8" s="7">
-        <f>-G8</f>
+        <f t="shared" si="1"/>
         <v>-92.710000000000008</v>
       </c>
     </row>
@@ -7411,15 +8880,15 @@
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7">
-        <f>B9*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>304.8</v>
       </c>
       <c r="G9" s="7">
-        <f>((C9*12)+D9)*2.54</f>
+        <f t="shared" si="2"/>
         <v>105.41</v>
       </c>
       <c r="H9" s="7">
-        <f>-G9</f>
+        <f t="shared" si="1"/>
         <v>-105.41</v>
       </c>
     </row>
@@ -7435,15 +8904,15 @@
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7">
-        <f>B10*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>457.2</v>
       </c>
       <c r="G10" s="7">
-        <f>((C10*12)+D10)*2.54</f>
+        <f t="shared" si="2"/>
         <v>116.84</v>
       </c>
       <c r="H10" s="7">
-        <f>-G10</f>
+        <f t="shared" si="1"/>
         <v>-116.84</v>
       </c>
     </row>
@@ -7459,15 +8928,15 @@
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7">
-        <f>B11*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>609.6</v>
       </c>
       <c r="G11" s="7">
-        <f>((C11*12)+D11)*2.54</f>
+        <f t="shared" si="2"/>
         <v>127</v>
       </c>
       <c r="H11" s="7">
-        <f>-G11</f>
+        <f t="shared" si="1"/>
         <v>-127</v>
       </c>
     </row>
@@ -7483,15 +8952,15 @@
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7">
-        <f>B12*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>670.56000000000006</v>
       </c>
       <c r="G12" s="7">
-        <f>((C12*12)+D12)*2.54</f>
+        <f t="shared" si="2"/>
         <v>130.81</v>
       </c>
       <c r="H12" s="7">
-        <f>-G12</f>
+        <f t="shared" si="1"/>
         <v>-130.81</v>
       </c>
     </row>
@@ -7510,15 +8979,15 @@
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7">
-        <f>B13*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>731.52</v>
       </c>
       <c r="G13" s="7">
-        <f>((C13*12)+D13)*2.54</f>
+        <f t="shared" si="2"/>
         <v>133.98500000000001</v>
       </c>
       <c r="H13" s="7">
-        <f>-G13</f>
+        <f t="shared" si="1"/>
         <v>-133.98500000000001</v>
       </c>
     </row>
@@ -7534,15 +9003,15 @@
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7">
-        <f>B14*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>762</v>
       </c>
       <c r="G14" s="7">
-        <f>((C14*12)+D14)*2.54</f>
+        <f t="shared" si="2"/>
         <v>137.16</v>
       </c>
       <c r="H14" s="7">
-        <f>-G14</f>
+        <f t="shared" si="1"/>
         <v>-137.16</v>
       </c>
     </row>
@@ -7558,15 +9027,15 @@
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7">
-        <f>B15*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>792.48</v>
       </c>
       <c r="G15" s="7">
-        <f>((C15*12)+D15)*2.54</f>
+        <f t="shared" si="2"/>
         <v>139.69999999999999</v>
       </c>
       <c r="H15" s="7">
-        <f>-G15</f>
+        <f t="shared" si="1"/>
         <v>-139.69999999999999</v>
       </c>
     </row>
@@ -7582,15 +9051,15 @@
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7">
-        <f>B16*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>822.96</v>
       </c>
       <c r="G16" s="7">
-        <f>((C16*12)+D16)*2.54</f>
+        <f t="shared" si="2"/>
         <v>141.60499999999999</v>
       </c>
       <c r="H16" s="7">
-        <f>-G16</f>
+        <f t="shared" si="1"/>
         <v>-141.60499999999999</v>
       </c>
     </row>
@@ -7606,15 +9075,15 @@
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7">
-        <f>B17*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>853.44</v>
       </c>
       <c r="G17" s="7">
-        <f>((C17*12)+D17)*2.54</f>
+        <f t="shared" si="2"/>
         <v>142.24</v>
       </c>
       <c r="H17" s="7">
-        <f>-G17</f>
+        <f t="shared" si="1"/>
         <v>-142.24</v>
       </c>
     </row>
@@ -7630,15 +9099,15 @@
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7">
-        <f>B18*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>883.92</v>
       </c>
       <c r="G18" s="7">
-        <f>((C18*12)+D18)*2.54</f>
+        <f t="shared" si="2"/>
         <v>140.97</v>
       </c>
       <c r="H18" s="7">
-        <f>-G18</f>
+        <f t="shared" si="1"/>
         <v>-140.97</v>
       </c>
     </row>
@@ -7654,15 +9123,15 @@
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7">
-        <f>B19*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>914.4</v>
       </c>
       <c r="G19" s="7">
-        <f>((C19*12)+D19)*2.54</f>
+        <f t="shared" si="2"/>
         <v>138.43</v>
       </c>
       <c r="H19" s="7">
-        <f>-G19</f>
+        <f t="shared" si="1"/>
         <v>-138.43</v>
       </c>
     </row>
@@ -7678,15 +9147,15 @@
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7">
-        <f>B20*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>944.88</v>
       </c>
       <c r="G20" s="7">
-        <f>((C20*12)+D20)*2.54</f>
+        <f t="shared" si="2"/>
         <v>137.16</v>
       </c>
       <c r="H20" s="7">
-        <f>-G20</f>
+        <f t="shared" si="1"/>
         <v>-137.16</v>
       </c>
     </row>
@@ -7705,15 +9174,15 @@
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7">
-        <f>B21*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>975.36</v>
       </c>
       <c r="G21" s="7">
-        <f>((C21*12)+D21)*2.54</f>
+        <f t="shared" si="2"/>
         <v>134.62</v>
       </c>
       <c r="H21" s="7">
-        <f>-G21</f>
+        <f t="shared" si="1"/>
         <v>-134.62</v>
       </c>
     </row>
@@ -7729,15 +9198,15 @@
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7">
-        <f>B22*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1036.32</v>
       </c>
       <c r="G22" s="7">
-        <f>((C22*12)+D22)*2.54</f>
+        <f t="shared" si="2"/>
         <v>130.17500000000001</v>
       </c>
       <c r="H22" s="7">
-        <f>-G22</f>
+        <f t="shared" si="1"/>
         <v>-130.17500000000001</v>
       </c>
     </row>
@@ -7753,15 +9222,15 @@
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7">
-        <f>B23*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1097.28</v>
       </c>
       <c r="G23" s="7">
-        <f>((C23*12)+D23)*2.54</f>
+        <f t="shared" si="2"/>
         <v>125.73</v>
       </c>
       <c r="H23" s="7">
-        <f>-G23</f>
+        <f t="shared" si="1"/>
         <v>-125.73</v>
       </c>
     </row>
@@ -7777,15 +9246,15 @@
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7">
-        <f>B24*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1158.24</v>
       </c>
       <c r="G24" s="7">
-        <f>((C24*12)+D24)*2.54</f>
+        <f t="shared" si="2"/>
         <v>121.92</v>
       </c>
       <c r="H24" s="7">
-        <f>-G24</f>
+        <f t="shared" si="1"/>
         <v>-121.92</v>
       </c>
     </row>
@@ -7801,15 +9270,15 @@
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7">
-        <f>B25*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1219.2</v>
       </c>
       <c r="G25" s="7">
-        <f>((C25*12)+D25)*2.54</f>
+        <f t="shared" si="2"/>
         <v>118.11</v>
       </c>
       <c r="H25" s="7">
-        <f>-G25</f>
+        <f t="shared" si="1"/>
         <v>-118.11</v>
       </c>
     </row>
@@ -7825,15 +9294,15 @@
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7">
-        <f>B26*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1280.1600000000001</v>
       </c>
       <c r="G26" s="7">
-        <f>((C26*12)+D26)*2.54</f>
+        <f t="shared" si="2"/>
         <v>114.935</v>
       </c>
       <c r="H26" s="7">
-        <f>-G26</f>
+        <f t="shared" si="1"/>
         <v>-114.935</v>
       </c>
     </row>
@@ -7849,15 +9318,15 @@
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7">
-        <f>B27*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1371.6</v>
       </c>
       <c r="G27" s="7">
-        <f>((C27*12)+D27)*2.54</f>
+        <f t="shared" si="2"/>
         <v>111.76</v>
       </c>
       <c r="H27" s="7">
-        <f>-G27</f>
+        <f t="shared" si="1"/>
         <v>-111.76</v>
       </c>
     </row>
@@ -7873,15 +9342,15 @@
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7">
-        <f>B28*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1524</v>
       </c>
       <c r="G28" s="7">
-        <f>((C28*12)+D28)*2.54</f>
+        <f t="shared" si="2"/>
         <v>93.98</v>
       </c>
       <c r="H28" s="7">
-        <f>-G28</f>
+        <f t="shared" si="1"/>
         <v>-93.98</v>
       </c>
     </row>
@@ -7897,15 +9366,15 @@
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7">
-        <f>B29*12*2.54</f>
+        <f t="shared" si="0"/>
         <v>1676.4</v>
       </c>
       <c r="G29" s="7">
-        <f>((C29*12)+D29)*2.54</f>
+        <f t="shared" si="2"/>
         <v>66.040000000000006</v>
       </c>
       <c r="H29" s="7">
-        <f>-G29</f>
+        <f t="shared" si="1"/>
         <v>-66.040000000000006</v>
       </c>
     </row>
@@ -7916,16 +9385,1129 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="4" width="10.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="21">
+        <v>1</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="21">
+        <v>2</v>
+      </c>
+      <c r="F1" s="22"/>
+      <c r="G1" s="21">
+        <v>3</v>
+      </c>
+      <c r="H1" s="22"/>
+      <c r="I1" s="21">
+        <v>4</v>
+      </c>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="15" t="s">
         <v>24</v>
       </c>
+      <c r="C2" s="23">
+        <v>4</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="23">
+        <v>3</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="23">
+        <v>2</v>
+      </c>
+      <c r="H2" s="24"/>
+      <c r="I2" s="23">
+        <v>1</v>
+      </c>
+      <c r="J2" s="24"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="18"/>
+      <c r="D4" s="19">
+        <f>'HEC3'!D3*12*2.54</f>
+        <v>1158.24</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19">
+        <f>'HEC2'!D3*12*2.54</f>
+        <v>2042.16</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19">
+        <f>'HEC1'!D3*12*2.54</f>
+        <v>3810</v>
+      </c>
+      <c r="I4" s="18">
+        <f>'DT Upstream'!D3*12*2.54</f>
+        <v>975.36</v>
+      </c>
+      <c r="J4" s="19">
+        <f>'DT Upstream'!E3*12*2.54</f>
+        <v>1417.32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="18">
+        <f>'HEC4'!F6</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="19">
+        <f>'HEC4'!H6</f>
+        <v>-66.040000000000006</v>
+      </c>
+      <c r="E6" s="18">
+        <f>'HEC3'!F6</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="19">
+        <f>'HEC3'!H6</f>
+        <v>8.89</v>
+      </c>
+      <c r="G6" s="18">
+        <f>'HEC2'!F6</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="19">
+        <f>'HEC2'!H6</f>
+        <v>-93.98</v>
+      </c>
+      <c r="I6" s="18">
+        <f>'HEC1'!F6</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="19">
+        <f>'HEC1'!H6</f>
+        <v>-159.38499999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="18">
+        <f>'HEC4'!F7</f>
+        <v>60.96</v>
+      </c>
+      <c r="D7" s="19">
+        <f>'HEC4'!H7</f>
+        <v>-86.36</v>
+      </c>
+      <c r="E7" s="18">
+        <f>'HEC3'!F7</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="19">
+        <f>'HEC3'!H7</f>
+        <v>-138.43</v>
+      </c>
+      <c r="G7" s="18">
+        <f>'HEC2'!F7</f>
+        <v>60.96</v>
+      </c>
+      <c r="H7" s="19">
+        <f>'HEC2'!H7</f>
+        <v>-121.92</v>
+      </c>
+      <c r="I7" s="18">
+        <f>'HEC1'!F7</f>
+        <v>60.96</v>
+      </c>
+      <c r="J7" s="19">
+        <f>'HEC1'!H7</f>
+        <v>-215.26499999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="18">
+        <f>'HEC4'!F8</f>
+        <v>121.92</v>
+      </c>
+      <c r="D8" s="19">
+        <f>'HEC4'!H8</f>
+        <v>-95.25</v>
+      </c>
+      <c r="E8" s="18">
+        <f>'HEC3'!F8</f>
+        <v>60.96</v>
+      </c>
+      <c r="F8" s="19">
+        <f>'HEC3'!H8</f>
+        <v>-154.94</v>
+      </c>
+      <c r="G8" s="18">
+        <f>'HEC2'!F8</f>
+        <v>121.92</v>
+      </c>
+      <c r="H8" s="19">
+        <f>'HEC2'!H8</f>
+        <v>-171.45</v>
+      </c>
+      <c r="I8" s="18">
+        <f>'HEC1'!F8</f>
+        <v>101.4984</v>
+      </c>
+      <c r="J8" s="19">
+        <f>'HEC1'!H8</f>
+        <v>-250.82499999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="18">
+        <f>'HEC4'!F9</f>
+        <v>144.78</v>
+      </c>
+      <c r="D9" s="19">
+        <f>'HEC4'!H9</f>
+        <v>-118.11</v>
+      </c>
+      <c r="E9" s="18">
+        <f>'HEC3'!F9</f>
+        <v>121.92</v>
+      </c>
+      <c r="F9" s="19">
+        <f>'HEC3'!H9</f>
+        <v>-168.91</v>
+      </c>
+      <c r="G9" s="18">
+        <f>'HEC2'!F9</f>
+        <v>182.88</v>
+      </c>
+      <c r="H9" s="19">
+        <f>'HEC2'!H9</f>
+        <v>-200.66</v>
+      </c>
+      <c r="I9" s="18">
+        <f>'HEC1'!F9</f>
+        <v>101.4984</v>
+      </c>
+      <c r="J9" s="19">
+        <f>'HEC1'!H9</f>
+        <v>-255.90500000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="18">
+        <f>'HEC4'!F10</f>
+        <v>144.78</v>
+      </c>
+      <c r="D10" s="19">
+        <f>'HEC4'!H10</f>
+        <v>-125.73</v>
+      </c>
+      <c r="E10" s="18">
+        <f>'HEC3'!F10</f>
+        <v>182.88</v>
+      </c>
+      <c r="F10" s="19">
+        <f>'HEC3'!H10</f>
+        <v>-176.53</v>
+      </c>
+      <c r="G10" s="18">
+        <f>'HEC2'!F10</f>
+        <v>192.93840000000003</v>
+      </c>
+      <c r="H10" s="19">
+        <f>'HEC2'!H10</f>
+        <v>-205.74</v>
+      </c>
+      <c r="I10" s="18">
+        <f>'HEC1'!F10</f>
+        <v>121.92</v>
+      </c>
+      <c r="J10" s="19">
+        <f>'HEC1'!H10</f>
+        <v>-258.44499999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="18">
+        <f>'HEC4'!F11</f>
+        <v>182.88</v>
+      </c>
+      <c r="D11" s="19">
+        <f>'HEC4'!H11</f>
+        <v>-122.55500000000001</v>
+      </c>
+      <c r="E11" s="18">
+        <f>'HEC3'!F11</f>
+        <v>243.84</v>
+      </c>
+      <c r="F11" s="19">
+        <f>'HEC3'!H11</f>
+        <v>-180.34</v>
+      </c>
+      <c r="G11" s="18">
+        <f>'HEC2'!F11</f>
+        <v>192.93840000000003</v>
+      </c>
+      <c r="H11" s="19">
+        <f>'HEC2'!H11</f>
+        <v>-185.42000000000002</v>
+      </c>
+      <c r="I11" s="18">
+        <f>'HEC1'!F11</f>
+        <v>182.88</v>
+      </c>
+      <c r="J11" s="19">
+        <f>'HEC1'!H11</f>
+        <v>-268.60500000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="18">
+        <f>'HEC4'!F12</f>
+        <v>243.84</v>
+      </c>
+      <c r="D12" s="19">
+        <f>'HEC4'!H12</f>
+        <v>-129.54</v>
+      </c>
+      <c r="E12" s="18">
+        <f>'HEC3'!F12</f>
+        <v>253.89840000000004</v>
+      </c>
+      <c r="F12" s="19">
+        <f>'HEC3'!H12</f>
+        <v>-186.69</v>
+      </c>
+      <c r="G12" s="18">
+        <f>'HEC2'!F12</f>
+        <v>243.84</v>
+      </c>
+      <c r="H12" s="19">
+        <f>'HEC2'!H12</f>
+        <v>-214.63</v>
+      </c>
+      <c r="I12" s="18">
+        <f>'HEC1'!F12</f>
+        <v>243.84</v>
+      </c>
+      <c r="J12" s="19">
+        <f>'HEC1'!H12</f>
+        <v>-266.065</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="18">
+        <f>'HEC4'!F13</f>
+        <v>304.8</v>
+      </c>
+      <c r="D13" s="19">
+        <f>'HEC4'!H13</f>
+        <v>-148.59</v>
+      </c>
+      <c r="E13" s="18">
+        <f>'HEC3'!F13</f>
+        <v>253.89840000000004</v>
+      </c>
+      <c r="F13" s="19">
+        <f>'HEC3'!H13</f>
+        <v>-193.04</v>
+      </c>
+      <c r="G13" s="18">
+        <f>'HEC2'!F13</f>
+        <v>304.8</v>
+      </c>
+      <c r="H13" s="19">
+        <f>'HEC2'!H13</f>
+        <v>-224.79</v>
+      </c>
+      <c r="I13" s="18">
+        <f>'HEC1'!F13</f>
+        <v>274.32</v>
+      </c>
+      <c r="J13" s="19">
+        <f>'HEC1'!H13</f>
+        <v>-250.82499999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="18">
+        <f>'HEC4'!F14</f>
+        <v>365.76</v>
+      </c>
+      <c r="D14" s="19">
+        <f>'HEC4'!H14</f>
+        <v>-128.27000000000001</v>
+      </c>
+      <c r="E14" s="18">
+        <f>'HEC3'!F14</f>
+        <v>304.8</v>
+      </c>
+      <c r="F14" s="19">
+        <f>'HEC3'!H14</f>
+        <v>-193.04</v>
+      </c>
+      <c r="G14" s="18">
+        <f>'HEC2'!F14</f>
+        <v>365.76</v>
+      </c>
+      <c r="H14" s="19">
+        <f>'HEC2'!H14</f>
+        <v>-210.82</v>
+      </c>
+      <c r="I14" s="18">
+        <f>'HEC1'!F14</f>
+        <v>304.8</v>
+      </c>
+      <c r="J14" s="19">
+        <f>'HEC1'!H14</f>
+        <v>-245.745</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="18">
+        <f>'HEC4'!F15</f>
+        <v>426.72</v>
+      </c>
+      <c r="D15" s="19">
+        <f>'HEC4'!H15</f>
+        <v>-144.78</v>
+      </c>
+      <c r="E15" s="18">
+        <f>'HEC3'!F15</f>
+        <v>365.76</v>
+      </c>
+      <c r="F15" s="19">
+        <f>'HEC3'!H15</f>
+        <v>-199.39000000000001</v>
+      </c>
+      <c r="G15" s="18">
+        <f>'HEC2'!F15</f>
+        <v>426.72</v>
+      </c>
+      <c r="H15" s="19">
+        <f>'HEC2'!H15</f>
+        <v>-185.42000000000002</v>
+      </c>
+      <c r="I15" s="18">
+        <f>'HEC1'!F15</f>
+        <v>365.76</v>
+      </c>
+      <c r="J15" s="19">
+        <f>'HEC1'!H15</f>
+        <v>-230.505</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="18">
+        <f>'HEC4'!F16</f>
+        <v>470.91599999999994</v>
+      </c>
+      <c r="D16" s="19">
+        <f>'HEC4'!H16</f>
+        <v>-132.08000000000001</v>
+      </c>
+      <c r="E16" s="18">
+        <f>'HEC3'!F16</f>
+        <v>373.38</v>
+      </c>
+      <c r="F16" s="19">
+        <f>'HEC3'!H16</f>
+        <v>-203.2</v>
+      </c>
+      <c r="G16" s="18">
+        <f>'HEC2'!F16</f>
+        <v>487.68</v>
+      </c>
+      <c r="H16" s="19">
+        <f>'HEC2'!H16</f>
+        <v>-157.47999999999999</v>
+      </c>
+      <c r="I16" s="18">
+        <f>'HEC1'!F16</f>
+        <v>426.72</v>
+      </c>
+      <c r="J16" s="19">
+        <f>'HEC1'!H16</f>
+        <v>-141.60500000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="18">
+        <f>'HEC4'!F17</f>
+        <v>470.91599999999994</v>
+      </c>
+      <c r="D17" s="19">
+        <f>'HEC4'!H17</f>
+        <v>-137.16</v>
+      </c>
+      <c r="E17" s="18">
+        <f>'HEC3'!F17</f>
+        <v>373.38</v>
+      </c>
+      <c r="F17" s="19">
+        <f>'HEC3'!H17</f>
+        <v>-185.42000000000002</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="18">
+        <f>'HEC1'!F17</f>
+        <v>487.68</v>
+      </c>
+      <c r="J17" s="19">
+        <f>'HEC1'!H17</f>
+        <v>-93.344999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="20">
+        <f>'HEC4'!F18</f>
+        <v>487.68</v>
+      </c>
+      <c r="D18" s="14">
+        <f>'HEC4'!H18</f>
+        <v>-134.62</v>
+      </c>
+      <c r="E18" s="20">
+        <f>'HEC3'!F18</f>
+        <v>401.11680000000007</v>
+      </c>
+      <c r="F18" s="14">
+        <f>'HEC3'!H18</f>
+        <v>-99.06</v>
+      </c>
+      <c r="G18" s="20"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="21">
+        <v>1</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="21">
+        <v>2</v>
+      </c>
+      <c r="F1" s="22"/>
+      <c r="G1" s="21">
+        <v>3</v>
+      </c>
+      <c r="H1" s="22"/>
+      <c r="I1" s="21">
+        <v>4</v>
+      </c>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="23">
+        <v>4</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="23">
+        <v>3</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="23">
+        <v>2</v>
+      </c>
+      <c r="H2" s="24"/>
+      <c r="I2" s="23">
+        <v>1</v>
+      </c>
+      <c r="J2" s="24"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="18"/>
+      <c r="D4" s="19">
+        <f>'HEC3'!D3*12*2.54/100</f>
+        <v>11.5824</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19">
+        <f>'HEC2'!D3*12*2.54/100</f>
+        <v>20.421600000000002</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19">
+        <f>'HEC1'!D3*12*2.54/100</f>
+        <v>38.1</v>
+      </c>
+      <c r="I4" s="18">
+        <f>'DT Upstream'!D3*12*2.54/100</f>
+        <v>9.7536000000000005</v>
+      </c>
+      <c r="J4" s="19">
+        <f>'DT Upstream'!E3*12*2.54/100</f>
+        <v>14.1732</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="18">
+        <f>Summary!C6/100</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="19">
+        <f>Summary!D6/100</f>
+        <v>-0.6604000000000001</v>
+      </c>
+      <c r="E6" s="18">
+        <f>Summary!E6/100</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="19">
+        <f>Summary!F6/100</f>
+        <v>8.8900000000000007E-2</v>
+      </c>
+      <c r="G6" s="18">
+        <f>Summary!G6/100</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="19">
+        <f>Summary!H6/100</f>
+        <v>-0.93980000000000008</v>
+      </c>
+      <c r="I6" s="18">
+        <f>Summary!I6/100</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="19">
+        <f>Summary!J6/100</f>
+        <v>-1.59385</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="18">
+        <f>Summary!C7/100</f>
+        <v>0.60960000000000003</v>
+      </c>
+      <c r="D7" s="19">
+        <f>Summary!D7/100</f>
+        <v>-0.86360000000000003</v>
+      </c>
+      <c r="E7" s="18">
+        <f>Summary!E7/100</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="19">
+        <f>Summary!F7/100</f>
+        <v>-1.3843000000000001</v>
+      </c>
+      <c r="G7" s="18">
+        <f>Summary!G7/100</f>
+        <v>0.60960000000000003</v>
+      </c>
+      <c r="H7" s="19">
+        <f>Summary!H7/100</f>
+        <v>-1.2192000000000001</v>
+      </c>
+      <c r="I7" s="18">
+        <f>Summary!I7/100</f>
+        <v>0.60960000000000003</v>
+      </c>
+      <c r="J7" s="19">
+        <f>Summary!J7/100</f>
+        <v>-2.15265</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="18">
+        <f>Summary!C8/100</f>
+        <v>1.2192000000000001</v>
+      </c>
+      <c r="D8" s="19">
+        <f>Summary!D8/100</f>
+        <v>-0.95250000000000001</v>
+      </c>
+      <c r="E8" s="18">
+        <f>Summary!E8/100</f>
+        <v>0.60960000000000003</v>
+      </c>
+      <c r="F8" s="19">
+        <f>Summary!F8/100</f>
+        <v>-1.5493999999999999</v>
+      </c>
+      <c r="G8" s="18">
+        <f>Summary!G8/100</f>
+        <v>1.2192000000000001</v>
+      </c>
+      <c r="H8" s="19">
+        <f>Summary!H8/100</f>
+        <v>-1.7144999999999999</v>
+      </c>
+      <c r="I8" s="18">
+        <f>Summary!I8/100</f>
+        <v>1.0149840000000001</v>
+      </c>
+      <c r="J8" s="19">
+        <f>Summary!J8/100</f>
+        <v>-2.5082499999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="18">
+        <f>Summary!C9/100</f>
+        <v>1.4478</v>
+      </c>
+      <c r="D9" s="19">
+        <f>Summary!D9/100</f>
+        <v>-1.1811</v>
+      </c>
+      <c r="E9" s="18">
+        <f>Summary!E9/100</f>
+        <v>1.2192000000000001</v>
+      </c>
+      <c r="F9" s="19">
+        <f>Summary!F9/100</f>
+        <v>-1.6891</v>
+      </c>
+      <c r="G9" s="18">
+        <f>Summary!G9/100</f>
+        <v>1.8288</v>
+      </c>
+      <c r="H9" s="19">
+        <f>Summary!H9/100</f>
+        <v>-2.0066000000000002</v>
+      </c>
+      <c r="I9" s="18">
+        <f>Summary!I9/100</f>
+        <v>1.0149840000000001</v>
+      </c>
+      <c r="J9" s="19">
+        <f>Summary!J9/100</f>
+        <v>-2.5590500000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="18">
+        <f>Summary!C10/100</f>
+        <v>1.4478</v>
+      </c>
+      <c r="D10" s="19">
+        <f>Summary!D10/100</f>
+        <v>-1.2573000000000001</v>
+      </c>
+      <c r="E10" s="18">
+        <f>Summary!E10/100</f>
+        <v>1.8288</v>
+      </c>
+      <c r="F10" s="19">
+        <f>Summary!F10/100</f>
+        <v>-1.7653000000000001</v>
+      </c>
+      <c r="G10" s="18">
+        <f>Summary!G10/100</f>
+        <v>1.9293840000000002</v>
+      </c>
+      <c r="H10" s="19">
+        <f>Summary!H10/100</f>
+        <v>-2.0573999999999999</v>
+      </c>
+      <c r="I10" s="18">
+        <f>Summary!I10/100</f>
+        <v>1.2192000000000001</v>
+      </c>
+      <c r="J10" s="19">
+        <f>Summary!J10/100</f>
+        <v>-2.5844499999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="18">
+        <f>Summary!C11/100</f>
+        <v>1.8288</v>
+      </c>
+      <c r="D11" s="19">
+        <f>Summary!D11/100</f>
+        <v>-1.2255500000000001</v>
+      </c>
+      <c r="E11" s="18">
+        <f>Summary!E11/100</f>
+        <v>2.4384000000000001</v>
+      </c>
+      <c r="F11" s="19">
+        <f>Summary!F11/100</f>
+        <v>-1.8034000000000001</v>
+      </c>
+      <c r="G11" s="18">
+        <f>Summary!G11/100</f>
+        <v>1.9293840000000002</v>
+      </c>
+      <c r="H11" s="19">
+        <f>Summary!H11/100</f>
+        <v>-1.8542000000000001</v>
+      </c>
+      <c r="I11" s="18">
+        <f>Summary!I11/100</f>
+        <v>1.8288</v>
+      </c>
+      <c r="J11" s="19">
+        <f>Summary!J11/100</f>
+        <v>-2.6860500000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="18">
+        <f>Summary!C12/100</f>
+        <v>2.4384000000000001</v>
+      </c>
+      <c r="D12" s="19">
+        <f>Summary!D12/100</f>
+        <v>-1.2953999999999999</v>
+      </c>
+      <c r="E12" s="18">
+        <f>Summary!E12/100</f>
+        <v>2.5389840000000006</v>
+      </c>
+      <c r="F12" s="19">
+        <f>Summary!F12/100</f>
+        <v>-1.8669</v>
+      </c>
+      <c r="G12" s="18">
+        <f>Summary!G12/100</f>
+        <v>2.4384000000000001</v>
+      </c>
+      <c r="H12" s="19">
+        <f>Summary!H12/100</f>
+        <v>-2.1463000000000001</v>
+      </c>
+      <c r="I12" s="18">
+        <f>Summary!I12/100</f>
+        <v>2.4384000000000001</v>
+      </c>
+      <c r="J12" s="19">
+        <f>Summary!J12/100</f>
+        <v>-2.66065</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="18">
+        <f>Summary!C13/100</f>
+        <v>3.048</v>
+      </c>
+      <c r="D13" s="19">
+        <f>Summary!D13/100</f>
+        <v>-1.4859</v>
+      </c>
+      <c r="E13" s="18">
+        <f>Summary!E13/100</f>
+        <v>2.5389840000000006</v>
+      </c>
+      <c r="F13" s="19">
+        <f>Summary!F13/100</f>
+        <v>-1.9303999999999999</v>
+      </c>
+      <c r="G13" s="18">
+        <f>Summary!G13/100</f>
+        <v>3.048</v>
+      </c>
+      <c r="H13" s="19">
+        <f>Summary!H13/100</f>
+        <v>-2.2479</v>
+      </c>
+      <c r="I13" s="18">
+        <f>Summary!I13/100</f>
+        <v>2.7431999999999999</v>
+      </c>
+      <c r="J13" s="19">
+        <f>Summary!J13/100</f>
+        <v>-2.5082499999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="18">
+        <f>Summary!C14/100</f>
+        <v>3.6576</v>
+      </c>
+      <c r="D14" s="19">
+        <f>Summary!D14/100</f>
+        <v>-1.2827000000000002</v>
+      </c>
+      <c r="E14" s="18">
+        <f>Summary!E14/100</f>
+        <v>3.048</v>
+      </c>
+      <c r="F14" s="19">
+        <f>Summary!F14/100</f>
+        <v>-1.9303999999999999</v>
+      </c>
+      <c r="G14" s="18">
+        <f>Summary!G14/100</f>
+        <v>3.6576</v>
+      </c>
+      <c r="H14" s="19">
+        <f>Summary!H14/100</f>
+        <v>-2.1082000000000001</v>
+      </c>
+      <c r="I14" s="18">
+        <f>Summary!I14/100</f>
+        <v>3.048</v>
+      </c>
+      <c r="J14" s="19">
+        <f>Summary!J14/100</f>
+        <v>-2.4574500000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="18">
+        <f>Summary!C15/100</f>
+        <v>4.2671999999999999</v>
+      </c>
+      <c r="D15" s="19">
+        <f>Summary!D15/100</f>
+        <v>-1.4478</v>
+      </c>
+      <c r="E15" s="18">
+        <f>Summary!E15/100</f>
+        <v>3.6576</v>
+      </c>
+      <c r="F15" s="19">
+        <f>Summary!F15/100</f>
+        <v>-1.9939000000000002</v>
+      </c>
+      <c r="G15" s="18">
+        <f>Summary!G15/100</f>
+        <v>4.2671999999999999</v>
+      </c>
+      <c r="H15" s="19">
+        <f>Summary!H15/100</f>
+        <v>-1.8542000000000001</v>
+      </c>
+      <c r="I15" s="18">
+        <f>Summary!I15/100</f>
+        <v>3.6576</v>
+      </c>
+      <c r="J15" s="19">
+        <f>Summary!J15/100</f>
+        <v>-2.30505</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="18">
+        <f>Summary!C16/100</f>
+        <v>4.7091599999999998</v>
+      </c>
+      <c r="D16" s="19">
+        <f>Summary!D16/100</f>
+        <v>-1.3208000000000002</v>
+      </c>
+      <c r="E16" s="18">
+        <f>Summary!E16/100</f>
+        <v>3.7338</v>
+      </c>
+      <c r="F16" s="19">
+        <f>Summary!F16/100</f>
+        <v>-2.032</v>
+      </c>
+      <c r="G16" s="18">
+        <f>Summary!G16/100</f>
+        <v>4.8768000000000002</v>
+      </c>
+      <c r="H16" s="19">
+        <f>Summary!H16/100</f>
+        <v>-1.5748</v>
+      </c>
+      <c r="I16" s="18">
+        <f>Summary!I16/100</f>
+        <v>4.2671999999999999</v>
+      </c>
+      <c r="J16" s="19">
+        <f>Summary!J16/100</f>
+        <v>-1.4160500000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="18">
+        <f>Summary!C17/100</f>
+        <v>4.7091599999999998</v>
+      </c>
+      <c r="D17" s="19">
+        <f>Summary!D17/100</f>
+        <v>-1.3715999999999999</v>
+      </c>
+      <c r="E17" s="18">
+        <f>Summary!E17/100</f>
+        <v>3.7338</v>
+      </c>
+      <c r="F17" s="19">
+        <f>Summary!F17/100</f>
+        <v>-1.8542000000000001</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="18">
+        <f>Summary!I17/100</f>
+        <v>4.8768000000000002</v>
+      </c>
+      <c r="J17" s="19">
+        <f>Summary!J17/100</f>
+        <v>-0.93345</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="20">
+        <f>Summary!C18/100</f>
+        <v>4.8768000000000002</v>
+      </c>
+      <c r="D18" s="14">
+        <f>Summary!D18/100</f>
+        <v>-1.3462000000000001</v>
+      </c>
+      <c r="E18" s="20">
+        <f>Summary!E18/100</f>
+        <v>4.0111680000000005</v>
+      </c>
+      <c r="F18" s="14">
+        <f>Summary!F18/100</f>
+        <v>-0.99060000000000004</v>
+      </c>
+      <c r="G18" s="20"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>